<commit_message>
added China dn Iran
</commit_message>
<xml_diff>
--- a/data/Countries.xlsx
+++ b/data/Countries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="253">
   <si>
     <t>GeoId</t>
   </si>
@@ -770,6 +770,12 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>CN</t>
   </si>
 </sst>
 </file>
@@ -1079,13 +1085,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1126,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -1140,7 +1146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
@@ -1184,7 +1190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
@@ -1228,7 +1234,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
@@ -1248,7 +1254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
@@ -1268,7 +1274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
@@ -1312,7 +1318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>23</v>
@@ -1356,7 +1362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>24</v>
@@ -1376,7 +1382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>25</v>
@@ -1396,7 +1402,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>26</v>
@@ -1416,7 +1422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>27</v>
@@ -1436,7 +1442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1460,7 +1466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>32</v>
@@ -1504,7 +1510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>33</v>
@@ -1524,7 +1530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>34</v>
@@ -1544,7 +1550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>35</v>
@@ -1564,7 +1570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -1588,7 +1594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>38</v>
@@ -1608,7 +1614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>39</v>
@@ -1628,7 +1634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>40</v>
@@ -1648,7 +1654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
@@ -1672,7 +1678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>43</v>
@@ -1692,7 +1698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
         <v>44</v>
@@ -1712,7 +1718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>45</v>
@@ -1732,7 +1738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
         <v>46</v>
@@ -1752,7 +1758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
         <v>47</v>
@@ -1772,7 +1778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
         <v>48</v>
@@ -1792,7 +1798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>49</v>
@@ -1812,7 +1818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
         <v>50</v>
@@ -1832,7 +1838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>51</v>
@@ -1853,7 +1859,9 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="3" t="s">
+        <v>252</v>
+      </c>
       <c r="B37" s="3" t="s">
         <v>52</v>
       </c>
@@ -1872,7 +1880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>53</v>
@@ -1892,7 +1900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
         <v>54</v>
@@ -1912,7 +1920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>55</v>
@@ -1932,7 +1940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
         <v>56</v>
@@ -1952,7 +1960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>57</v>
@@ -1972,7 +1980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
         <v>58</v>
@@ -1992,7 +2000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>59</v>
       </c>
@@ -2016,7 +2024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>61</v>
@@ -2036,7 +2044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>62</v>
       </c>
@@ -2060,7 +2068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>64</v>
       </c>
@@ -2084,7 +2092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>66</v>
       </c>
@@ -2108,7 +2116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
         <v>68</v>
@@ -2128,7 +2136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
         <v>69</v>
@@ -2148,7 +2156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
         <v>70</v>
@@ -2168,7 +2176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
         <v>71</v>
@@ -2188,7 +2196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
         <v>72</v>
@@ -2208,7 +2216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3" t="s">
         <v>73</v>
@@ -2228,7 +2236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3" t="s">
         <v>74</v>
@@ -2248,7 +2256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3" t="s">
         <v>75</v>
@@ -2268,7 +2276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>76</v>
       </c>
@@ -2292,7 +2300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3" t="s">
         <v>78</v>
@@ -2312,7 +2320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3" t="s">
         <v>79</v>
@@ -2332,7 +2340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>80</v>
       </c>
@@ -2356,7 +2364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>82</v>
       </c>
@@ -2380,7 +2388,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
         <v>85</v>
@@ -2400,7 +2408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3" t="s">
         <v>86</v>
@@ -2420,7 +2428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>87</v>
       </c>
@@ -2444,7 +2452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>89</v>
       </c>
@@ -2468,7 +2476,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3" t="s">
         <v>91</v>
@@ -2488,7 +2496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>92</v>
       </c>
@@ -2512,7 +2520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3" t="s">
         <v>94</v>
@@ -2532,7 +2540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3" t="s">
         <v>95</v>
@@ -2552,7 +2560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3" t="s">
         <v>96</v>
@@ -2572,7 +2580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3" t="s">
         <v>97</v>
@@ -2592,7 +2600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3" t="s">
         <v>98</v>
@@ -2612,7 +2620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3" t="s">
         <v>99</v>
@@ -2632,7 +2640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3" t="s">
         <v>100</v>
@@ -2652,7 +2660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>101</v>
       </c>
@@ -2676,7 +2684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>103</v>
       </c>
@@ -2700,7 +2708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3" t="s">
         <v>105</v>
@@ -2720,7 +2728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3" t="s">
         <v>106</v>
@@ -2740,8 +2748,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
+    <row r="79" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="B79" s="3" t="s">
         <v>107</v>
       </c>
@@ -2760,7 +2770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3" t="s">
         <v>108</v>
@@ -2780,7 +2790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>109</v>
       </c>
@@ -2804,7 +2814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3" t="s">
         <v>111</v>
@@ -2824,7 +2834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>112</v>
       </c>
@@ -2848,7 +2858,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3" t="s">
         <v>114</v>
@@ -2868,7 +2878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3" t="s">
         <v>115</v>
@@ -2888,7 +2898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3" t="s">
         <v>116</v>
@@ -2908,7 +2918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3" t="s">
         <v>117</v>
@@ -2928,7 +2938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3" t="s">
         <v>118</v>
@@ -2948,7 +2958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3" t="s">
         <v>119</v>
@@ -2968,7 +2978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3" t="s">
         <v>120</v>
@@ -2988,7 +2998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3" t="s">
         <v>121</v>
@@ -3008,7 +3018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>122</v>
       </c>
@@ -3032,7 +3042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3" t="s">
         <v>124</v>
@@ -3052,7 +3062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3" t="s">
         <v>125</v>
@@ -3072,7 +3082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3" t="s">
         <v>126</v>
@@ -3092,7 +3102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>127</v>
       </c>
@@ -3116,7 +3126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3" t="s">
         <v>129</v>
@@ -3136,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3" t="s">
         <v>130</v>
@@ -3156,7 +3166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3" t="s">
         <v>131</v>
@@ -3176,7 +3186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3" t="s">
         <v>132</v>
@@ -3196,7 +3206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>133</v>
       </c>
@@ -3220,7 +3230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>135</v>
       </c>
@@ -3244,7 +3254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>137</v>
       </c>
@@ -3268,7 +3278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>139</v>
       </c>
@@ -3292,7 +3302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3" t="s">
         <v>141</v>
@@ -3312,7 +3322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3" t="s">
         <v>142</v>
@@ -3332,7 +3342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3" t="s">
         <v>143</v>
@@ -3352,7 +3362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3" t="s">
         <v>144</v>
@@ -3372,7 +3382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3" t="s">
         <v>145</v>
@@ -3392,7 +3402,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>146</v>
       </c>
@@ -3416,7 +3426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3" t="s">
         <v>148</v>
@@ -3436,7 +3446,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3" t="s">
         <v>149</v>
@@ -3456,7 +3466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3" t="s">
         <v>150</v>
@@ -3476,7 +3486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3" t="s">
         <v>151</v>
@@ -3496,7 +3506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3" t="s">
         <v>152</v>
@@ -3516,7 +3526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3" t="s">
         <v>153</v>
@@ -3536,7 +3546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>154</v>
       </c>
@@ -3560,7 +3570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3" t="s">
         <v>156</v>
@@ -3580,7 +3590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3" t="s">
         <v>157</v>
@@ -3600,7 +3610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3" t="s">
         <v>158</v>
@@ -3620,7 +3630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3" t="s">
         <v>159</v>
@@ -3640,7 +3650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3" t="s">
         <v>160</v>
@@ -3660,7 +3670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3" t="s">
         <v>161</v>
@@ -3680,7 +3690,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3" t="s">
         <v>162</v>
@@ -3700,7 +3710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3" t="s">
         <v>163</v>
@@ -3720,7 +3730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>164</v>
       </c>
@@ -3744,7 +3754,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
         <v>166</v>
@@ -3764,7 +3774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
         <v>167</v>
@@ -3784,7 +3794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
         <v>168</v>
@@ -3804,7 +3814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
         <v>169</v>
@@ -3824,7 +3834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>170</v>
       </c>
@@ -3848,7 +3858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
         <v>172</v>
@@ -3868,7 +3878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3" t="s">
         <v>173</v>
@@ -3888,7 +3898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
         <v>174</v>
@@ -3908,7 +3918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
         <v>175</v>
@@ -3928,7 +3938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
         <v>176</v>
@@ -3948,7 +3958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3" t="s">
         <v>177</v>
@@ -3968,7 +3978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3" t="s">
         <v>178</v>
@@ -3988,7 +3998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3" t="s">
         <v>179</v>
@@ -4008,7 +4018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>180</v>
       </c>
@@ -4032,7 +4042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>182</v>
       </c>
@@ -4056,7 +4066,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3" t="s">
         <v>184</v>
@@ -4076,7 +4086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>185</v>
       </c>
@@ -4100,7 +4110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>187</v>
       </c>
@@ -4124,7 +4134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="3" t="s">
         <v>189</v>
@@ -4144,7 +4154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="3" t="s">
         <v>190</v>
@@ -4164,7 +4174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="3" t="s">
         <v>191</v>
@@ -4184,7 +4194,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="3" t="s">
         <v>192</v>
@@ -4204,7 +4214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="3" t="s">
         <v>193</v>
@@ -4224,7 +4234,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="3" t="s">
         <v>194</v>
@@ -4244,7 +4254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3" t="s">
         <v>195</v>
@@ -4264,7 +4274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3" t="s">
         <v>196</v>
@@ -4284,7 +4294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3" t="s">
         <v>197</v>
@@ -4304,7 +4314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3" t="s">
         <v>198</v>
@@ -4324,7 +4334,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="3" t="s">
         <v>199</v>
@@ -4344,7 +4354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="3" t="s">
         <v>200</v>
@@ -4364,7 +4374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="3" t="s">
         <v>201</v>
@@ -4384,7 +4394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>202</v>
       </c>
@@ -4408,7 +4418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>204</v>
       </c>
@@ -4432,7 +4442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="3" t="s">
         <v>206</v>
@@ -4452,7 +4462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
       <c r="B161" s="3" t="s">
         <v>207</v>
@@ -4472,7 +4482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
       <c r="B162" s="3" t="s">
         <v>208</v>
@@ -4492,7 +4502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="3" t="s">
         <v>209</v>
@@ -4512,7 +4522,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>210</v>
       </c>
@@ -4536,7 +4546,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="3" t="s">
         <v>212</v>
@@ -4556,7 +4566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="3" t="s">
         <v>213</v>
@@ -4576,7 +4586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="3" t="s">
         <v>214</v>
@@ -4596,7 +4606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="3" t="s">
         <v>215</v>
@@ -4616,7 +4626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>216</v>
       </c>
@@ -4640,7 +4650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>218</v>
       </c>
@@ -4664,7 +4674,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
       <c r="B171" s="3" t="s">
         <v>220</v>
@@ -4684,7 +4694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
       <c r="B172" s="3" t="s">
         <v>221</v>
@@ -4704,7 +4714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="3" t="s">
         <v>222</v>
@@ -4724,7 +4734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
       <c r="B174" s="3" t="s">
         <v>223</v>
@@ -4744,7 +4754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="3" t="s">
         <v>224</v>
@@ -4764,7 +4774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="3" t="s">
         <v>225</v>
@@ -4784,7 +4794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="3" t="s">
         <v>226</v>
@@ -4804,7 +4814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="3" t="s">
         <v>227</v>
@@ -4824,7 +4834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="3" t="s">
         <v>228</v>
@@ -4844,7 +4854,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="3" t="s">
         <v>229</v>
@@ -4864,7 +4874,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
       <c r="B181" s="3" t="s">
         <v>230</v>
@@ -4884,7 +4894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="3" t="s">
         <v>231</v>
@@ -4904,7 +4914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="3" t="s">
         <v>232</v>
@@ -4924,7 +4934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
       <c r="B184" s="3" t="s">
         <v>233</v>
@@ -4944,7 +4954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>234</v>
       </c>
@@ -4968,7 +4978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
       <c r="B186" s="3" t="s">
         <v>236</v>
@@ -4988,7 +4998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>237</v>
       </c>
@@ -5012,7 +5022,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
       <c r="B188" s="3" t="s">
         <v>239</v>
@@ -5032,7 +5042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
       <c r="B189" s="3" t="s">
         <v>240</v>
@@ -5052,7 +5062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="3" t="s">
         <v>241</v>
@@ -5072,7 +5082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
       <c r="B191" s="3" t="s">
         <v>242</v>
@@ -5092,7 +5102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>243</v>
       </c>
@@ -5116,7 +5126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
       <c r="B193" s="3" t="s">
         <v>245</v>
@@ -5136,7 +5146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
       <c r="B194" s="3" t="s">
         <v>246</v>
@@ -5156,7 +5166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
       <c r="B195" s="3" t="s">
         <v>247</v>
@@ -5176,7 +5186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
       <c r="B196" s="3" t="s">
         <v>248</v>
@@ -5196,7 +5206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
       <c r="B197" s="3" t="s">
         <v>249</v>
@@ -5216,7 +5226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="3" t="s">
         <v>250</v>
@@ -10049,7 +10059,13 @@
       <c r="G1000" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G198"/>
+  <autoFilter ref="B1:G198">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="China"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>